<commit_message>
bj: update of the forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Benin/2023/bj_sch_sth_impact_202304_2_child.xlsx
+++ b/SCH-STH/Impact assessments/Benin/2023/bj_sch_sth_impact_202304_2_child.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\SCH-STH\Impact assessments\Benin\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\dsa-forms\SCH-STH\Impact assessments\Benin\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D27F850-7F21-46E1-8886-B01ED995055F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64618655-F09F-4314-B1CE-2ED58DAC5748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="245">
   <si>
     <t>type</t>
   </si>
@@ -541,15 +541,6 @@
     <t>Select the school</t>
   </si>
   <si>
-    <t>p_affections</t>
-  </si>
-  <si>
-    <t>Affections ciblées pour évaluation dans la commune</t>
-  </si>
-  <si>
-    <t>Targeted diseases for evaluation in the commune</t>
-  </si>
-  <si>
     <t>Enter the participant's order number</t>
   </si>
   <si>
@@ -794,9 +785,6 @@
   </si>
   <si>
     <t>concat(${p_site_code},'-',if(${num}&lt;10, concat('0', ${num}), ${num}))</t>
-  </si>
-  <si>
-    <t>select_one affections_list</t>
   </si>
   <si>
     <t>affections_list</t>
@@ -1363,34 +1351,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15.625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="42.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="41.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="19.59765625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="42.59765625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="41.19921875" style="4" customWidth="1"/>
     <col min="5" max="5" width="47.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="47.375" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="16.875" customWidth="1"/>
+    <col min="6" max="6" width="47.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.59765625" customWidth="1"/>
+    <col min="8" max="8" width="16.8984375" customWidth="1"/>
     <col min="9" max="10" width="29.5" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="12.625" customWidth="1"/>
-    <col min="13" max="13" width="9.75" customWidth="1"/>
-    <col min="14" max="14" width="13.875" customWidth="1"/>
-    <col min="15" max="15" width="36.625" customWidth="1"/>
+    <col min="12" max="12" width="12.59765625" customWidth="1"/>
+    <col min="13" max="13" width="9.69921875" customWidth="1"/>
+    <col min="14" max="14" width="13.8984375" customWidth="1"/>
+    <col min="15" max="15" width="36.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="19" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
@@ -1437,10 +1425,10 @@
         <v>14</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="5" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
@@ -1448,26 +1436,26 @@
         <v>15</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="24" t="s">
         <v>221</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>224</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -1477,7 +1465,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
@@ -1504,7 +1492,7 @@
       <c r="N3" s="9"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
@@ -1530,15 +1518,15 @@
       </c>
       <c r="N4" s="9"/>
       <c r="O4" s="38" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>157</v>
@@ -1559,33 +1547,33 @@
       </c>
       <c r="N5" s="9"/>
       <c r="O5" s="38" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="36" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="35" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F6" s="35"/>
       <c r="G6" s="8"/>
       <c r="H6" s="9" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -1594,23 +1582,15 @@
       </c>
       <c r="N6" s="9"/>
       <c r="O6" s="38" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>243</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>160</v>
-      </c>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="11" t="s">
-        <v>159</v>
-      </c>
+      <c r="E7" s="11"/>
       <c r="F7" s="11"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -1618,18 +1598,24 @@
       <c r="J7" s="11"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="30" t="s">
-        <v>16</v>
-      </c>
+      <c r="M7" s="30"/>
       <c r="N7" s="9"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="29"/>
+    <row r="8" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>192</v>
+      </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
+      <c r="E8" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="F8" s="11"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -1641,19 +1627,19 @@
       <c r="N8" s="9"/>
       <c r="O8" s="8"/>
     </row>
-    <row r="9" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="36" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>195</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="8"/>
@@ -1662,108 +1648,110 @@
       <c r="J9" s="11"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
-      <c r="M9" s="30"/>
+      <c r="M9" s="30" t="s">
+        <v>16</v>
+      </c>
       <c r="N9" s="9"/>
       <c r="O9" s="8"/>
     </row>
-    <row r="10" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="36" t="s">
-        <v>172</v>
+        <v>196</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="11" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="10"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="9"/>
+      <c r="K10" s="36" t="s">
+        <v>199</v>
+      </c>
       <c r="L10" s="9"/>
-      <c r="M10" s="30" t="s">
-        <v>16</v>
-      </c>
+      <c r="M10" s="30"/>
       <c r="N10" s="9"/>
       <c r="O10" s="8"/>
     </row>
-    <row r="11" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
-        <v>199</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>203</v>
-      </c>
+    <row r="11" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="36"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="11" t="s">
-        <v>200</v>
-      </c>
+      <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="10"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="36" t="s">
-        <v>202</v>
-      </c>
+      <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="30"/>
       <c r="N11" s="9"/>
       <c r="O11" s="8"/>
     </row>
-    <row r="12" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="29"/>
+    <row r="12" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>158</v>
+      </c>
       <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>238</v>
+      </c>
       <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="11"/>
+      <c r="H12" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="I12" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="J12" s="35" t="s">
+        <v>216</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
-      <c r="M12" s="30"/>
+      <c r="M12" s="30" t="s">
+        <v>16</v>
+      </c>
       <c r="N12" s="9"/>
       <c r="O12" s="8"/>
     </row>
-    <row r="13" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36" t="s">
-        <v>30</v>
+    <row r="13" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>161</v>
       </c>
       <c r="D13" s="10"/>
-      <c r="E13" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>241</v>
-      </c>
+      <c r="E13" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="F13" s="11"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="37" t="s">
-        <v>236</v>
-      </c>
-      <c r="I13" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="J13" s="35" t="s">
-        <v>219</v>
-      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="11"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="30" t="s">
@@ -1772,19 +1760,19 @@
       <c r="N13" s="9"/>
       <c r="O13" s="8"/>
     </row>
-    <row r="14" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
-        <v>162</v>
+        <v>34</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>207</v>
+        <v>70</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="31" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="8"/>
@@ -1799,20 +1787,12 @@
       <c r="N14" s="9"/>
       <c r="O14" s="8"/>
     </row>
-    <row r="15" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>35</v>
-      </c>
+    <row r="15" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="10"/>
-      <c r="E15" s="31" t="s">
-        <v>36</v>
-      </c>
+      <c r="E15" s="31"/>
       <c r="F15" s="11"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -1820,53 +1800,69 @@
       <c r="J15" s="11"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
-      <c r="M15" s="30" t="s">
-        <v>16</v>
-      </c>
+      <c r="M15" s="30"/>
       <c r="N15" s="9"/>
       <c r="O15" s="8"/>
     </row>
-    <row r="16" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="11"/>
+    <row r="16" spans="1:16" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="10"/>
       <c r="J16" s="11"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
-      <c r="M16" s="30"/>
+      <c r="M16" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="N16" s="9"/>
       <c r="O16" s="8"/>
     </row>
-    <row r="17" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>25</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D17" s="10"/>
       <c r="E17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>27</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F17" s="11"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="9"/>
+      <c r="H17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>223</v>
+      </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9" t="s">
         <v>16</v>
@@ -1874,54 +1870,48 @@
       <c r="N17" s="9"/>
       <c r="O17" s="8"/>
     </row>
-    <row r="18" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>209</v>
+        <v>169</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>207</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>31</v>
+        <v>170</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="11" t="s">
-        <v>32</v>
+      <c r="E18" s="31" t="s">
+        <v>171</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>235</v>
-      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="11"/>
       <c r="K18" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L18" s="9"/>
-      <c r="M18" s="9" t="s">
+      <c r="M18" s="30" t="s">
         <v>16</v>
       </c>
       <c r="N18" s="9"/>
       <c r="O18" s="8"/>
     </row>
-    <row r="19" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>173</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="8"/>
@@ -1929,76 +1919,64 @@
       <c r="I19" s="10"/>
       <c r="J19" s="11"/>
       <c r="K19" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="L19" s="9"/>
-      <c r="M19" s="30" t="s">
-        <v>16</v>
-      </c>
+      <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="8"/>
     </row>
-    <row r="20" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>172</v>
+    <row r="20" spans="1:16" s="19" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="40" t="s">
+        <v>29</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>211</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>176</v>
+        <v>209</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>175</v>
       </c>
       <c r="D20" s="10"/>
-      <c r="E20" s="31" t="s">
-        <v>175</v>
+      <c r="E20" s="35" t="s">
+        <v>174</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
       <c r="I20" s="10"/>
       <c r="J20" s="11"/>
       <c r="K20" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
+        <v>223</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="M20" s="30" t="s">
+        <v>16</v>
+      </c>
       <c r="N20" s="9"/>
       <c r="O20" s="8"/>
-    </row>
-    <row r="21" spans="1:16" s="19" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>212</v>
-      </c>
-      <c r="C21" s="34" t="s">
-        <v>178</v>
-      </c>
+      <c r="P20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="10"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="35" t="s">
-        <v>177</v>
-      </c>
+      <c r="E21" s="31"/>
       <c r="F21" s="11"/>
       <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="10"/>
       <c r="J21" s="11"/>
-      <c r="K21" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="L21" s="9" t="s">
-        <v>242</v>
-      </c>
-      <c r="M21" s="30" t="s">
-        <v>16</v>
-      </c>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="8"/>
-      <c r="P21" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
       <c r="B22" s="30"/>
       <c r="C22" s="10"/>
@@ -2015,48 +1993,60 @@
       <c r="N22" s="9"/>
       <c r="O22" s="8"/>
     </row>
-    <row r="23" spans="1:16" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="11"/>
+    <row r="23" spans="1:16" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="L23" s="8"/>
+      <c r="M23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N23" s="8"/>
       <c r="O23" s="8"/>
     </row>
-    <row r="24" spans="1:16" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="19" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>38</v>
-      </c>
+      <c r="D24" s="10"/>
       <c r="E24" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>40</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F24" s="11"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="26"/>
       <c r="J24" s="27"/>
-      <c r="K24" s="8" t="s">
-        <v>227</v>
+      <c r="K24" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="L24" s="8"/>
       <c r="M24" s="9" t="s">
@@ -2065,19 +2055,19 @@
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:16" s="19" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="19" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>214</v>
+        <v>137</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="11" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="8"/>
@@ -2085,88 +2075,86 @@
       <c r="I25" s="26"/>
       <c r="J25" s="27"/>
       <c r="K25" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L25" s="8"/>
-      <c r="M25" s="9" t="s">
-        <v>16</v>
-      </c>
+      <c r="M25" s="9"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8"/>
     </row>
-    <row r="26" spans="1:16" s="19" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="19" customFormat="1" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>137</v>
+        <v>212</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="27"/>
+      <c r="H26" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>48</v>
+      </c>
       <c r="K26" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L26" s="8"/>
       <c r="M26" s="9"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8"/>
     </row>
-    <row r="27" spans="1:16" s="19" customFormat="1" ht="63" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="J27" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="L27" s="8"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-    </row>
-    <row r="28" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="1:16" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D28" s="23"/>
       <c r="E28" s="25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="12"/>
@@ -2174,54 +2162,44 @@
       <c r="I28" s="13"/>
       <c r="J28" s="14"/>
       <c r="K28" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
       <c r="O28" s="12"/>
     </row>
-    <row r="29" spans="1:16" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
       <c r="I29" s="13"/>
       <c r="J29" s="14"/>
-      <c r="K29" s="8" t="s">
-        <v>231</v>
-      </c>
+      <c r="K29" s="8"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
       <c r="O29" s="12"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C30" s="23" t="s">
-        <v>53</v>
-      </c>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="23"/>
       <c r="D30" s="23"/>
-      <c r="E30" s="25" t="s">
-        <v>54</v>
-      </c>
+      <c r="E30" s="25"/>
       <c r="F30" s="14"/>
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
@@ -2233,8 +2211,10 @@
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="39" t="s">
+        <v>201</v>
+      </c>
       <c r="B31" s="22"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
@@ -2250,9 +2230,9 @@
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="39" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B32" s="22"/>
       <c r="C32" s="23"/>
@@ -2269,12 +2249,16 @@
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
-        <v>205</v>
-      </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>57</v>
+      </c>
       <c r="D33" s="23"/>
       <c r="E33" s="25"/>
       <c r="F33" s="14"/>
@@ -2288,12 +2272,12 @@
       <c r="N33" s="12"/>
       <c r="O33" s="12"/>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>55</v>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>57</v>
@@ -2311,29 +2295,6 @@
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B35" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2346,19 +2307,19 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49:XFD428"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="40" style="5" customWidth="1"/>
-    <col min="4" max="4" width="46.125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="4" max="4" width="46.09765625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="15.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>60</v>
       </c>
@@ -2372,19 +2333,19 @@
         <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2394,45 +2355,45 @@
       <c r="G2" s="18"/>
       <c r="H2" s="18"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="17"/>
       <c r="G3" s="18"/>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
         <v>61</v>
       </c>
@@ -2446,7 +2407,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>61</v>
       </c>
@@ -2460,13 +2421,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>66</v>
       </c>
@@ -2480,7 +2441,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>66</v>
       </c>
@@ -2494,7 +2455,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>70</v>
       </c>
@@ -2508,7 +2469,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>70</v>
       </c>
@@ -2522,7 +2483,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>76</v>
       </c>
@@ -2536,7 +2497,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>76</v>
       </c>
@@ -2550,7 +2511,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>76</v>
       </c>
@@ -2564,7 +2525,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>76</v>
       </c>
@@ -2578,7 +2539,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>76</v>
       </c>
@@ -2592,7 +2553,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
         <v>76</v>
       </c>
@@ -2606,7 +2567,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>94</v>
       </c>
@@ -2620,7 +2581,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
         <v>94</v>
       </c>
@@ -2634,7 +2595,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>94</v>
       </c>
@@ -2648,7 +2609,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>101</v>
       </c>
@@ -2662,7 +2623,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
         <v>101</v>
       </c>
@@ -2676,7 +2637,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
         <v>101</v>
       </c>
@@ -2690,7 +2651,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>111</v>
       </c>
@@ -2704,7 +2665,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
         <v>111</v>
       </c>
@@ -2718,7 +2679,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>111</v>
       </c>
@@ -2732,7 +2693,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
         <v>111</v>
       </c>
@@ -2746,7 +2707,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
         <v>111</v>
       </c>
@@ -2760,7 +2721,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
         <v>111</v>
       </c>
@@ -2774,7 +2735,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>111</v>
       </c>
@@ -2788,7 +2749,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>130</v>
       </c>
@@ -2802,7 +2763,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>130</v>
       </c>
@@ -2816,7 +2777,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>137</v>
       </c>
@@ -2830,7 +2791,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>137</v>
       </c>
@@ -2844,7 +2805,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -2858,7 +2819,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>137</v>
       </c>
@@ -2872,7 +2833,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -2886,7 +2847,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -2900,88 +2861,88 @@
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" s="33" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="C44" s="33" t="s">
+        <v>165</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="C42" s="33" t="s">
+      <c r="C45" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="D42" s="33" t="s">
+      <c r="D45" s="33" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="B43" s="33" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C46" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D46" s="33" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="B44" s="33" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C47" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="D44" s="33" t="s">
+      <c r="D47" s="33" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="B45" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="C45" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="D45" s="33" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="B46" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="D46" s="33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="B47" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="C47" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2995,17 +2956,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.125" customWidth="1"/>
-    <col min="2" max="2" width="32.125" customWidth="1"/>
+    <col min="1" max="1" width="44.09765625" customWidth="1"/>
+    <col min="2" max="2" width="32.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>150</v>
       </c>
@@ -3016,12 +2977,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
         <v>153</v>

</xml_diff>